<commit_message>
mi primer commit a learning
</commit_message>
<xml_diff>
--- a/data/udf/Formato1_Excel_Reservas.xlsx
+++ b/data/udf/Formato1_Excel_Reservas.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10720"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arquitecturaml/Documents/ITMEET/Operaciones/Client/Hydroginc/BP010-data-pipelines/data/udf/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ITMeet\Operaciones\BP010-data-pipelines-auditoria\data\udf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD62B6DD-CAE5-F049-AD37-A21EB87F08DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1F22162-DDD2-43DA-949F-B8CC00ABCC4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="26880" windowHeight="16800" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Datos Maestros" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Datos Maestros'!$A$1:$S$1</definedName>
   </definedNames>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="191028" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -95,7 +95,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="74">
   <si>
     <t>ID</t>
   </si>
@@ -308,6 +308,15 @@
   </si>
   <si>
     <t>State Blanco 58 A003</t>
+  </si>
+  <si>
+    <t>Rod Weight In Air, Lb</t>
+  </si>
+  <si>
+    <t>API Maximum Fluid Load, Lb</t>
+  </si>
+  <si>
+    <t>Reserva inicial teorica</t>
   </si>
 </sst>
 </file>
@@ -316,9 +325,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="169" formatCode="0.0000"/>
+    <numFmt numFmtId="165" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -338,12 +347,14 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Aptos Narrow"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Aptos Narrow"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -364,8 +375,22 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u val="singleAccounting"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -384,6 +409,12 @@
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -397,7 +428,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment readingOrder="1"/>
@@ -436,11 +467,26 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -825,21 +871,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S42"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="172" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="172" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.5" style="2"/>
-    <col min="2" max="2" width="14.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="35.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.44140625" style="2"/>
+    <col min="2" max="2" width="14.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.44140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="32" style="7" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15.6640625" customWidth="1"/>
-    <col min="10" max="10" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -868,7 +914,7 @@
       <c r="R1" s="1"/>
       <c r="S1" s="1"/>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -897,7 +943,7 @@
       <c r="R2" s="1"/>
       <c r="S2" s="1"/>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -926,7 +972,7 @@
       <c r="R3" s="1"/>
       <c r="S3" s="1"/>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -955,7 +1001,7 @@
       <c r="R4" s="1"/>
       <c r="S4" s="1"/>
     </row>
-    <row r="5" spans="1:19" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:19" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -984,7 +1030,7 @@
       <c r="R5" s="1"/>
       <c r="S5" s="1"/>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -1013,7 +1059,7 @@
       <c r="R6" s="1"/>
       <c r="S6" s="1"/>
     </row>
-    <row r="7" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>12</v>
       </c>
@@ -1042,7 +1088,7 @@
       <c r="R7" s="1"/>
       <c r="S7" s="1"/>
     </row>
-    <row r="8" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>13</v>
       </c>
@@ -1071,7 +1117,7 @@
       <c r="R8" s="1"/>
       <c r="S8" s="1"/>
     </row>
-    <row r="9" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:19" s="2" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>14</v>
       </c>
@@ -1100,7 +1146,7 @@
       <c r="R9" s="1"/>
       <c r="S9" s="1"/>
     </row>
-    <row r="10" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:19" s="3" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>15</v>
       </c>
@@ -1129,7 +1175,7 @@
       <c r="R10" s="1"/>
       <c r="S10" s="1"/>
     </row>
-    <row r="11" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>16</v>
       </c>
@@ -1158,7 +1204,7 @@
       <c r="R11" s="1"/>
       <c r="S11" s="1"/>
     </row>
-    <row r="12" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>17</v>
       </c>
@@ -1187,7 +1233,7 @@
       <c r="R12" s="1"/>
       <c r="S12" s="1"/>
     </row>
-    <row r="13" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>19</v>
       </c>
@@ -1216,7 +1262,7 @@
       <c r="R13" s="1"/>
       <c r="S13" s="1"/>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>20</v>
       </c>
@@ -1245,7 +1291,7 @@
       <c r="R14" s="1"/>
       <c r="S14" s="1"/>
     </row>
-    <row r="15" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <v>21</v>
       </c>
@@ -1274,7 +1320,7 @@
       <c r="R15" s="1"/>
       <c r="S15" s="1"/>
     </row>
-    <row r="16" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <v>22</v>
       </c>
@@ -1303,7 +1349,7 @@
       <c r="R16" s="1"/>
       <c r="S16" s="1"/>
     </row>
-    <row r="17" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <v>23</v>
       </c>
@@ -1332,7 +1378,7 @@
       <c r="R17" s="1"/>
       <c r="S17" s="1"/>
     </row>
-    <row r="18" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
         <v>26</v>
       </c>
@@ -1361,7 +1407,7 @@
       <c r="R18" s="1"/>
       <c r="S18" s="1"/>
     </row>
-    <row r="19" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
         <v>28</v>
       </c>
@@ -1390,7 +1436,7 @@
       <c r="R19" s="1"/>
       <c r="S19" s="1"/>
     </row>
-    <row r="20" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
         <v>33</v>
       </c>
@@ -1419,7 +1465,7 @@
       <c r="R20" s="1"/>
       <c r="S20" s="1"/>
     </row>
-    <row r="21" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
         <v>37</v>
       </c>
@@ -1448,7 +1494,7 @@
       <c r="R21" s="1"/>
       <c r="S21" s="1"/>
     </row>
-    <row r="22" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
         <v>38</v>
       </c>
@@ -1477,7 +1523,7 @@
       <c r="R22" s="1"/>
       <c r="S22" s="1"/>
     </row>
-    <row r="23" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="2">
         <v>39</v>
       </c>
@@ -1506,7 +1552,7 @@
       <c r="R23" s="1"/>
       <c r="S23" s="1"/>
     </row>
-    <row r="24" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="2">
         <v>42</v>
       </c>
@@ -1535,7 +1581,7 @@
       <c r="R24" s="1"/>
       <c r="S24" s="1"/>
     </row>
-    <row r="25" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="2">
         <v>43</v>
       </c>
@@ -1564,7 +1610,7 @@
       <c r="R25" s="1"/>
       <c r="S25" s="1"/>
     </row>
-    <row r="26" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="2">
         <v>44</v>
       </c>
@@ -1593,7 +1639,7 @@
       <c r="R26" s="1"/>
       <c r="S26" s="1"/>
     </row>
-    <row r="27" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="2">
         <v>45</v>
       </c>
@@ -1622,7 +1668,7 @@
       <c r="R27" s="1"/>
       <c r="S27" s="1"/>
     </row>
-    <row r="28" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="2">
         <v>46</v>
       </c>
@@ -1651,7 +1697,7 @@
       <c r="R28" s="1"/>
       <c r="S28" s="1"/>
     </row>
-    <row r="29" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="2">
         <v>47</v>
       </c>
@@ -1680,7 +1726,7 @@
       <c r="R29" s="1"/>
       <c r="S29" s="1"/>
     </row>
-    <row r="30" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="2">
         <v>49</v>
       </c>
@@ -1709,7 +1755,7 @@
       <c r="R30" s="1"/>
       <c r="S30" s="1"/>
     </row>
-    <row r="31" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="2">
         <v>85</v>
       </c>
@@ -1738,7 +1784,7 @@
       <c r="R31" s="1"/>
       <c r="S31" s="1"/>
     </row>
-    <row r="32" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="2">
         <v>87</v>
       </c>
@@ -1767,9 +1813,19 @@
       <c r="R32" s="1"/>
       <c r="S32" s="1"/>
     </row>
-    <row r="33" spans="3:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C33" s="1"/>
-      <c r="D33" s="6"/>
+    <row r="33" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="19">
+        <v>72</v>
+      </c>
+      <c r="B33" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="C33" s="20" t="s">
+        <v>71</v>
+      </c>
+      <c r="D33" s="21">
+        <v>22500</v>
+      </c>
       <c r="E33" s="1"/>
       <c r="F33" s="1"/>
       <c r="G33" s="1"/>
@@ -1786,9 +1842,19 @@
       <c r="R33" s="1"/>
       <c r="S33" s="1"/>
     </row>
-    <row r="34" spans="3:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C34" s="1"/>
-      <c r="D34" s="6"/>
+    <row r="34" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="19">
+        <v>75</v>
+      </c>
+      <c r="B34" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="C34" s="22" t="s">
+        <v>72</v>
+      </c>
+      <c r="D34" s="21">
+        <v>2250</v>
+      </c>
       <c r="E34" s="1"/>
       <c r="F34" s="1"/>
       <c r="G34" s="1"/>
@@ -1805,7 +1871,7 @@
       <c r="R34" s="1"/>
       <c r="S34" s="1"/>
     </row>
-    <row r="35" spans="3:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C35" s="1"/>
       <c r="D35" s="6"/>
       <c r="E35" s="1"/>
@@ -1824,7 +1890,7 @@
       <c r="R35" s="1"/>
       <c r="S35" s="1"/>
     </row>
-    <row r="36" spans="3:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C36" s="1"/>
       <c r="D36" s="6"/>
       <c r="E36" s="1"/>
@@ -1843,7 +1909,7 @@
       <c r="R36" s="1"/>
       <c r="S36" s="1"/>
     </row>
-    <row r="37" spans="3:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C37" s="1"/>
       <c r="D37" s="6"/>
       <c r="E37" s="1"/>
@@ -1862,7 +1928,7 @@
       <c r="R37" s="1"/>
       <c r="S37" s="1"/>
     </row>
-    <row r="38" spans="3:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C38" s="1"/>
       <c r="D38" s="6"/>
       <c r="E38" s="1"/>
@@ -1881,7 +1947,7 @@
       <c r="R38" s="1"/>
       <c r="S38" s="1"/>
     </row>
-    <row r="39" spans="3:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C39" s="1"/>
       <c r="D39" s="6"/>
       <c r="E39" s="1"/>
@@ -1900,7 +1966,7 @@
       <c r="R39" s="1"/>
       <c r="S39" s="1"/>
     </row>
-    <row r="40" spans="3:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C40" s="1"/>
       <c r="D40" s="6"/>
       <c r="E40" s="1"/>
@@ -1919,7 +1985,7 @@
       <c r="R40" s="1"/>
       <c r="S40" s="1"/>
     </row>
-    <row r="41" spans="3:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C41" s="1"/>
       <c r="D41" s="6"/>
       <c r="E41" s="1"/>
@@ -1938,7 +2004,7 @@
       <c r="R41" s="1"/>
       <c r="S41" s="1"/>
     </row>
-    <row r="42" spans="3:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C42" s="1"/>
       <c r="D42" s="6"/>
       <c r="E42" s="1"/>
@@ -1967,21 +2033,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FBC1AE4-91CA-4177-A5F3-8C6B6DFB1C67}">
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="279" workbookViewId="0">
+    <sheetView topLeftCell="A16" zoomScale="279" workbookViewId="0">
       <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.44140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="34.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.5" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.21875" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
@@ -1995,7 +2061,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2009,7 +2075,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>10</v>
       </c>
@@ -2023,7 +2089,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>18</v>
       </c>
@@ -2037,7 +2103,7 @@
         <v>0.76</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>24</v>
       </c>
@@ -2051,7 +2117,7 @@
         <v>4010</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>25</v>
       </c>
@@ -2065,7 +2131,7 @@
         <v>4010</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>27</v>
       </c>
@@ -2079,7 +2145,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>29</v>
       </c>
@@ -2093,7 +2159,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>30</v>
       </c>
@@ -2107,7 +2173,7 @@
         <v>1.1294</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>32</v>
       </c>
@@ -2121,7 +2187,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>48</v>
       </c>
@@ -2135,7 +2201,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>58</v>
       </c>
@@ -2149,7 +2215,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>59</v>
       </c>
@@ -2163,7 +2229,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>63</v>
       </c>
@@ -2177,7 +2243,7 @@
         <v>1.05</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>152</v>
       </c>
@@ -2191,7 +2257,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>159</v>
       </c>
@@ -2205,7 +2271,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>160</v>
       </c>
@@ -2219,7 +2285,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>161</v>
       </c>
@@ -2233,7 +2299,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>162</v>
       </c>
@@ -2246,6 +2312,23 @@
       <c r="D19" s="4">
         <v>0</v>
       </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="24">
+        <v>128</v>
+      </c>
+      <c r="B20" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="C20" s="24" t="s">
+        <v>73</v>
+      </c>
+      <c r="D20" s="25">
+        <v>1250222</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="16.2" x14ac:dyDescent="0.45">
+      <c r="D21" s="23"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2254,38 +2337,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="a73fcaab-45e3-44dc-9856-f67638302e46" xsi:nil="true"/>
-    <Estadoderevisi_x00f3_n xmlns="a4041966-1e7c-4993-86fd-93921d09913a" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="a4041966-1e7c-4993-86fd-93921d09913a">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <Fechaderevisi_x00f3_n xmlns="a4041966-1e7c-4993-86fd-93921d09913a" xsi:nil="true"/>
-    <Imagen xmlns="a4041966-1e7c-4993-86fd-93921d09913a" xsi:nil="true"/>
-    <Estadodeaprobaci_x00f3_n xmlns="a4041966-1e7c-4993-86fd-93921d09913a">true</Estadodeaprobaci_x00f3_n>
-    <Accesorio_x002f_Parte xmlns="a4041966-1e7c-4993-86fd-93921d09913a" xsi:nil="true"/>
-    <Aprobador xmlns="a4041966-1e7c-4993-86fd-93921d09913a">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Aprobador>
-    <Observaciones xmlns="a4041966-1e7c-4993-86fd-93921d09913a" xsi:nil="true"/>
-    <Responsable xmlns="a4041966-1e7c-4993-86fd-93921d09913a">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Responsable>
-    <Aclaraciones xmlns="a4041966-1e7c-4993-86fd-93921d09913a" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100ED302B7ED0375B4E9E3810ECE8D59334" ma:contentTypeVersion="24" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e5bec10da2468dd28a979ec34a0e6a53">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="a4041966-1e7c-4993-86fd-93921d09913a" xmlns:ns3="a73fcaab-45e3-44dc-9856-f67638302e46" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="54bc646419bad60665844cbcd38a1cdc" ns2:_="" ns3:_="">
     <xsd:import namespace="a4041966-1e7c-4993-86fd-93921d09913a"/>
@@ -2612,6 +2663,38 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="a73fcaab-45e3-44dc-9856-f67638302e46" xsi:nil="true"/>
+    <Estadoderevisi_x00f3_n xmlns="a4041966-1e7c-4993-86fd-93921d09913a" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="a4041966-1e7c-4993-86fd-93921d09913a">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <Fechaderevisi_x00f3_n xmlns="a4041966-1e7c-4993-86fd-93921d09913a" xsi:nil="true"/>
+    <Imagen xmlns="a4041966-1e7c-4993-86fd-93921d09913a" xsi:nil="true"/>
+    <Estadodeaprobaci_x00f3_n xmlns="a4041966-1e7c-4993-86fd-93921d09913a">true</Estadodeaprobaci_x00f3_n>
+    <Accesorio_x002f_Parte xmlns="a4041966-1e7c-4993-86fd-93921d09913a" xsi:nil="true"/>
+    <Aprobador xmlns="a4041966-1e7c-4993-86fd-93921d09913a">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Aprobador>
+    <Observaciones xmlns="a4041966-1e7c-4993-86fd-93921d09913a" xsi:nil="true"/>
+    <Responsable xmlns="a4041966-1e7c-4993-86fd-93921d09913a">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Responsable>
+    <Aclaraciones xmlns="a4041966-1e7c-4993-86fd-93921d09913a" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -2622,17 +2705,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FE4F609A-FFF8-4169-BA2A-003C02215731}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="a73fcaab-45e3-44dc-9856-f67638302e46"/>
-    <ds:schemaRef ds:uri="a4041966-1e7c-4993-86fd-93921d09913a"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E81D4A7D-CA2D-4A21-BEFE-9B0404C48A3D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2651,6 +2723,17 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FE4F609A-FFF8-4169-BA2A-003C02215731}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="a73fcaab-45e3-44dc-9856-f67638302e46"/>
+    <ds:schemaRef ds:uri="a4041966-1e7c-4993-86fd-93921d09913a"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FDF2AD9E-CEFB-44A9-B8FC-F2507741A733}">
   <ds:schemaRefs>

</xml_diff>